<commit_message>
CRIANCA_HOSP change in model sheet
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B864527-7298-4DDA-A462-B95F596EBD5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9820CEB5-D1CC-418B-B9CC-C9C57BD2EBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="138">
   <si>
     <t>setting_name</t>
   </si>
@@ -402,9 +402,6 @@
     <t>informador</t>
   </si>
   <si>
-    <t>infporq</t>
-  </si>
-  <si>
     <t>Special information - why was the interview not possible</t>
   </si>
   <si>
@@ -432,9 +429,6 @@
     <t>data('informador') =='2'</t>
   </si>
   <si>
-    <t>infquem</t>
-  </si>
-  <si>
     <t>Who?</t>
   </si>
   <si>
@@ -442,6 +436,15 @@
   </si>
   <si>
     <t>REGIDC</t>
+  </si>
+  <si>
+    <t>INFORMADOR</t>
+  </si>
+  <si>
+    <t>INFPORQ</t>
+  </si>
+  <si>
+    <t>INFQUEM</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1031,8 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,10 +1093,10 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
         <v>122</v>
@@ -1108,7 +1111,7 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1117,13 +1120,13 @@
         <v>50</v>
       </c>
       <c r="F5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
         <v>133</v>
-      </c>
-      <c r="G5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1138,7 +1141,7 @@
         <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1147,13 +1150,13 @@
         <v>50</v>
       </c>
       <c r="F8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" t="s">
         <v>123</v>
       </c>
-      <c r="G8" t="s">
-        <v>124</v>
-      </c>
       <c r="H8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1856,62 +1859,62 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1926,7 +1929,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2062,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -2070,7 +2073,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>50</v>
@@ -2081,7 +2084,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
@@ -2136,7 +2139,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Added: Healthcenter dropdown in HOSP + logic for control-visits in MIF
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF920D0F-A29D-4232-8203-E9C006D93B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595C41D8-E8D3-4075-8C0C-ECC99FD27AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="150">
   <si>
     <t>setting_name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>begin screen</t>
   </si>
   <si>
-    <t>choice_item.REG === data('REG')</t>
-  </si>
-  <si>
     <t>uri</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>Date of hospitalisation</t>
   </si>
   <si>
-    <t>Code of place of hospitalisation</t>
-  </si>
-  <si>
     <t>DATAINT</t>
   </si>
   <si>
@@ -372,15 +366,6 @@
     <t>VISITIDC</t>
   </si>
   <si>
-    <t>HospCode</t>
-  </si>
-  <si>
-    <t>Facility 1</t>
-  </si>
-  <si>
-    <t>Facility 2</t>
-  </si>
-  <si>
     <t>informador</t>
   </si>
   <si>
@@ -429,9 +414,6 @@
     <t>Porque não foi possível a entrevista</t>
   </si>
   <si>
-    <t>Código de local de hospitalização</t>
-  </si>
-  <si>
     <t>Viu documentacão da data de internamento?</t>
   </si>
   <si>
@@ -448,6 +430,68 @@
   </si>
   <si>
     <t>Éra trauma/accidente</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>"HEALTHCENTRES.csv"</t>
+  </si>
+  <si>
+    <t>_.map(context, function(place){place.data_value = place.cscode;
+place.display = {title: {text: place.csname} };
+return place;
+})</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>select_one_dropdown</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
+    <t>choice_item.reg === data('reg')</t>
+  </si>
+  <si>
+    <t>region_csv</t>
+  </si>
+  <si>
+    <t>hc_csv</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Local de hospitalização</t>
+  </si>
+  <si>
+    <t>_.chain(context)
+.uniq(function(x) {
+return x.reg
+})
+.map(function(place){
+return {
+data_value:place.reg,
+display:{title: {text: place.regname} } };
+}).value()</t>
+  </si>
+  <si>
+    <t>Region: {{data.reg}}</t>
+  </si>
+  <si>
+    <t>Região: {{data.reg}}</t>
+  </si>
+  <si>
+    <t>Health center / hospital: {{data.ONDEINTC}}</t>
+  </si>
+  <si>
+    <t>Centro de saúde / hospital: {{data.ONDEINTC}}</t>
   </si>
 </sst>
 </file>
@@ -598,7 +642,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -611,7 +655,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -956,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,10 +1023,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,15 +1088,16 @@
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -1084,547 +1128,581 @@
       <c r="J1" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="D3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+        <v>69</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+        <v>102</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
       <c r="B13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+        <v>69</v>
+      </c>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
       <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="D16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" t="s">
+        <v>146</v>
+      </c>
+      <c r="H16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="D17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" t="s">
+        <v>148</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="D23" t="s">
         <v>22</v>
       </c>
-      <c r="E15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" t="s">
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="25"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" t="s">
+      <c r="E28" s="5"/>
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="24"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="24"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="D21" t="s">
+      <c r="H34" s="24"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="D35" t="s">
         <v>22</v>
       </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="25" t="s">
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="25" t="s">
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36" s="24"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" t="s">
+        <v>86</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" t="s">
+      <c r="H38" s="24"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" t="s">
+      <c r="H39" s="24"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="H26" s="25"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="D27" t="s">
+      <c r="H40" s="24"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="D41" t="s">
         <v>22</v>
       </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="D29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" t="s">
+      <c r="E41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" t="s">
+      <c r="H43" s="24"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" t="s">
         <v>46</v>
       </c>
-      <c r="H32" s="25"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="D33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="D35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" t="s">
-        <v>88</v>
-      </c>
-      <c r="G35" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="25"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="H38" s="25"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="D39" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" t="s">
-        <v>93</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" t="s">
-        <v>91</v>
-      </c>
-      <c r="H40" s="25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="H41" s="25"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="H42" s="25"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="D43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" t="s">
-        <v>95</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H43" s="25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" t="s">
-        <v>97</v>
-      </c>
-      <c r="H44" s="25"/>
+      <c r="H44" s="24"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>54</v>
       </c>
       <c r="F45" t="s">
-        <v>98</v>
-      </c>
-      <c r="G45" t="s">
-        <v>96</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>89</v>
+        <v>94</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" t="s">
-        <v>69</v>
-      </c>
-      <c r="H46" s="25"/>
+        <v>63</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H46" s="24"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" t="s">
-        <v>70</v>
-      </c>
-      <c r="H47" s="25"/>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" t="s">
+        <v>95</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="6"/>
       <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" s="24"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+      <c r="H49" s="24"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" t="s">
         <v>46</v>
       </c>
-      <c r="H48" s="25"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="D49" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="H50" s="24"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G51" t="s">
+        <v>98</v>
+      </c>
+      <c r="H51" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" t="s">
+        <v>101</v>
+      </c>
+      <c r="G52" t="s">
         <v>100</v>
       </c>
-      <c r="G49" t="s">
-        <v>99</v>
-      </c>
-      <c r="H49" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="D50" t="s">
-        <v>22</v>
-      </c>
-      <c r="E50" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" t="s">
-        <v>102</v>
-      </c>
-      <c r="G50" t="s">
-        <v>101</v>
-      </c>
-      <c r="H50" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" t="s">
-        <v>70</v>
+      <c r="H52" s="24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1638,22 +1716,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="58" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1685,34 +1764,52 @@
         <v>40</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
       <c r="C2"/>
       <c r="D2"/>
-      <c r="H2" s="10"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K5" s="13"/>
+      <c r="K5" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1755,27 +1852,27 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1785,11 +1882,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,47 +1913,47 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,62 +1988,32 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B7" t="str">
-        <f>"1"</f>
-        <v>1</v>
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B8" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" t="s">
-        <v>122</v>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1961,7 +2028,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +2051,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -1995,7 +2062,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -2006,10 +2073,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2017,10 +2084,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -2028,7 +2095,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -2039,7 +2106,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -2050,7 +2117,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -2061,10 +2128,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2072,7 +2139,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -2083,10 +2150,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -2094,7 +2161,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -2105,10 +2172,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2116,10 +2183,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -2127,10 +2194,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -2138,10 +2205,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>138</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2149,10 +2216,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2160,7 +2227,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -2171,10 +2238,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>50</v>
+        <v>122</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2182,10 +2249,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2193,36 +2260,44 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
+      <c r="B25" s="10"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="B26" s="10"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
+      <c r="B27" s="13"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
+      <c r="B28" s="10"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:C22">

</xml_diff>

<commit_message>
All kinds of changes from field tests
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72C25CB-31A7-42CD-8A9A-C4FFD4CED7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D1FFD0-3DFF-4BA0-BFEE-1C7CFD17B0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="159">
   <si>
     <t>setting_name</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>choice_item.reg === data('reg')</t>
-  </si>
-  <si>
-    <t>region_csv</t>
   </si>
   <si>
     <t>hc_csv</t>
@@ -494,15 +491,9 @@
     <t>Centro de saúde / hospital: {{data.ONDEINTC}}</t>
   </si>
   <si>
-    <t>data('ONDEINTC') == '9999'</t>
-  </si>
-  <si>
     <t>select_multiple</t>
   </si>
   <si>
-    <t>dontknow</t>
-  </si>
-  <si>
     <t>ondeintcns</t>
   </si>
   <si>
@@ -510,6 +501,24 @@
   </si>
   <si>
     <t>assign</t>
+  </si>
+  <si>
+    <t>reg_csv</t>
+  </si>
+  <si>
+    <t>dontknowfac</t>
+  </si>
+  <si>
+    <t>Other place</t>
+  </si>
+  <si>
+    <t>Outro lugar</t>
+  </si>
+  <si>
+    <t>data('ondeintcns')</t>
+  </si>
+  <si>
+    <t>data('ONDEINTC') == '8888'</t>
   </si>
 </sst>
 </file>
@@ -1095,9 +1104,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,13 +1293,13 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" t="s">
         <v>75</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1299,16 +1308,16 @@
         <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
         <v>136</v>
       </c>
       <c r="G16" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" t="s">
         <v>146</v>
-      </c>
-      <c r="H16" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1317,16 +1326,16 @@
         <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
       </c>
       <c r="G17" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" s="24" t="s">
         <v>148</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>149</v>
       </c>
       <c r="K17" s="11" t="s">
         <v>140</v>
@@ -1335,13 +1344,13 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H18" s="24"/>
       <c r="K18" s="11"/>
@@ -1352,7 +1361,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H19" s="24"/>
       <c r="K19" s="11"/>
@@ -1360,14 +1369,14 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F20" t="s">
         <v>104</v>
       </c>
       <c r="H20" s="24"/>
-      <c r="I20">
-        <v>9999</v>
+      <c r="I20" t="s">
+        <v>157</v>
       </c>
       <c r="K20" s="11"/>
     </row>
@@ -1392,7 +1401,7 @@
         <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H23" s="24"/>
     </row>
@@ -1799,9 +1808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,7 +1864,7 @@
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
         <v>133</v>
@@ -1871,12 +1880,12 @@
         <v>134</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
         <v>133</v>
@@ -1965,11 +1974,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="A9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,16 +2110,31 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B9" t="str">
+        <f>"8888"</f>
+        <v>8888</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" t="str">
         <f>"9999"</f>
         <v>9999</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2124,9 +2148,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,10 +2404,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
CONSTRAINTS Merge CRIANCA, CRIANCA_HOSP, GRAVIDA_VISIT
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D1FFD0-3DFF-4BA0-BFEE-1C7CFD17B0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13F1440-9D32-4109-9C88-6B9D0AD24DEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10380" yWindow="0" windowWidth="10395" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="164">
   <si>
     <t>setting_name</t>
   </si>
@@ -519,6 +519,21 @@
   </si>
   <si>
     <t>data('ONDEINTC') == '8888'</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text.english</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('CONT'), data('DATAINT'))&lt;0 || data('DATAINT') == null</t>
+  </si>
+  <si>
+    <t>Date of hospitalisation cannot be in the future</t>
   </si>
 </sst>
 </file>
@@ -1102,11 +1117,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,9 +1137,11 @@
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -1158,14 +1175,23 @@
       <c r="K1" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="D3" t="s">
         <v>22</v>
@@ -1183,7 +1209,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>63</v>
@@ -1193,7 +1219,7 @@
       </c>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="D5" t="s">
         <v>49</v>
@@ -1208,14 +1234,14 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>68</v>
       </c>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
         <v>63</v>
@@ -1225,7 +1251,7 @@
       </c>
       <c r="H7" s="24"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="D8" t="s">
         <v>49</v>
@@ -1240,28 +1266,28 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>68</v>
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>69</v>
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="D12" t="s">
         <v>60</v>
@@ -1275,22 +1301,31 @@
       <c r="H12" s="24" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>162</v>
+      </c>
+      <c r="M12" t="s">
+        <v>163</v>
+      </c>
+      <c r="N12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" t="s">
         <v>69</v>
       </c>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="D15" t="s">
         <v>142</v>
@@ -1302,7 +1337,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="D16" t="s">
         <v>138</v>
@@ -1976,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="A9:D10"/>
     </sheetView>

</xml_diff>

<commit_message>
Adding header + comment field in surveys
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4977A26B-7240-43B1-A562-658B3F5F89AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADDB341-AE94-425C-8CC1-0CECA8025DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="survey" sheetId="2" r:id="rId2"/>
-    <sheet name="queries" sheetId="6" r:id="rId3"/>
-    <sheet name="prompt_types" sheetId="5" r:id="rId4"/>
-    <sheet name="choices" sheetId="3" r:id="rId5"/>
-    <sheet name="model" sheetId="4" r:id="rId6"/>
+    <sheet name="calculates" sheetId="7" r:id="rId3"/>
+    <sheet name="queries" sheetId="6" r:id="rId4"/>
+    <sheet name="prompt_types" sheetId="5" r:id="rId5"/>
+    <sheet name="choices" sheetId="3" r:id="rId6"/>
+    <sheet name="model" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="174">
   <si>
     <t>setting_name</t>
   </si>
@@ -535,6 +536,36 @@
   <si>
     <t>CRIANCA</t>
   </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Comentário</t>
+  </si>
+  <si>
+    <t>OBSHOSP</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>outdate</t>
+  </si>
+  <si>
+    <t>calculation_name</t>
+  </si>
+  <si>
+    <t>displayOutdate</t>
+  </si>
+  <si>
+    <t>adate.display(data('outdate'))</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Hospitalization: {{data.nome}} - Dob: {{calculates.displayOutdate}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Hospitalizcao: {{data.nome}} - Nas: {{calculates.displayOutdate}}&lt;b&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -543,7 +574,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-406]General"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +630,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -707,11 +745,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{C28CC074-D3A0-48A2-81F3-B6A5CA836B7C}"/>
@@ -1113,11 +1151,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" activeCellId="1" sqref="F3:F58 D3:D58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,431 +1227,427 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
       <c r="D3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>112</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>122</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H4" s="21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="22"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="D5" t="s">
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="22"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" t="s">
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="D8" t="s">
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>123</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H9" s="21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" t="s">
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="22"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="D12" t="s">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" t="s">
+        <v>172</v>
+      </c>
+      <c r="H13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
         <v>103</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G14" t="s">
         <v>102</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H14" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L14" t="s">
         <v>161</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M14" t="s">
         <v>156</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" t="s">
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="D15" t="s">
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>140</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
+        <v>172</v>
+      </c>
+      <c r="H17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="D18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="D16" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="D19" t="s">
         <v>136</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E19" t="s">
         <v>147</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F19" t="s">
         <v>135</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G19" t="s">
         <v>157</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H19" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="D17" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="D20" t="s">
         <v>136</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E20" t="s">
         <v>139</v>
-      </c>
-      <c r="F17" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" t="s">
-        <v>159</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="D18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" t="s">
-        <v>148</v>
-      </c>
-      <c r="F18" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" t="s">
-        <v>145</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="D20" t="s">
-        <v>146</v>
       </c>
       <c r="F20" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" t="s">
+      <c r="G20" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="D21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="D23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" t="s">
         <v>151</v>
       </c>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" t="s">
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="K21" s="10"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" t="s">
+      <c r="H24" s="21"/>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" t="s">
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>152</v>
       </c>
-      <c r="H23" s="22"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" t="s">
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="D25" t="s">
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="D29" t="s">
         <v>49</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F29" t="s">
         <v>105</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G29" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H29" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="10"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" t="s">
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="22"/>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" t="s">
+      <c r="H30" s="21"/>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="D29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>65</v>
-      </c>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="D31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>67</v>
-      </c>
+      <c r="H31" s="21"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" t="s">
+        <v>172</v>
+      </c>
+      <c r="H33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" t="s">
+        <v>76</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" t="s">
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="D35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" t="s">
-        <v>73</v>
-      </c>
-      <c r="G35" t="s">
-        <v>78</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="22"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="D37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" t="s">
-        <v>80</v>
-      </c>
-      <c r="G37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
-      <c r="H38" s="22"/>
+      <c r="H38" s="21"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" t="s">
-        <v>69</v>
-      </c>
-      <c r="H39" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="H39" s="21"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-      <c r="H40" s="22"/>
+      <c r="D40" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" t="s">
+        <v>172</v>
+      </c>
+      <c r="H40" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
       <c r="D41" t="s">
         <v>22</v>
       </c>
@@ -1621,81 +1655,70 @@
         <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>82</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>127</v>
+        <v>78</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
       <c r="B42" t="s">
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H42" s="22"/>
+        <v>74</v>
+      </c>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
       <c r="D43" t="s">
         <v>49</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
       <c r="B44" t="s">
         <v>68</v>
       </c>
-      <c r="H44" s="22"/>
+      <c r="H44" s="21"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="15"/>
       <c r="B45" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="22"/>
+      <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="16"/>
       <c r="B46" t="s">
         <v>46</v>
       </c>
-      <c r="H46" s="22"/>
+      <c r="H46" s="21"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
       <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F47" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H47" s="22" t="s">
-        <v>128</v>
+        <v>140</v>
+      </c>
+      <c r="G47" t="s">
+        <v>172</v>
+      </c>
+      <c r="H47" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
       <c r="D48" t="s">
         <v>22</v>
       </c>
@@ -1703,129 +1726,255 @@
         <v>54</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G48" t="s">
-        <v>90</v>
-      </c>
-      <c r="H48" s="22" t="s">
-        <v>129</v>
+        <v>82</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
       <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" t="s">
+        <v>86</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51" s="21"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" t="s">
         <v>69</v>
       </c>
-      <c r="H49" s="22"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" t="s">
-        <v>46</v>
-      </c>
-      <c r="H50" s="22"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="D51" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" t="s">
-        <v>54</v>
-      </c>
-      <c r="F51" t="s">
-        <v>94</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H51" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" t="s">
-        <v>96</v>
-      </c>
-      <c r="H52" s="22"/>
+      <c r="H52" s="21"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
-      <c r="D53" t="s">
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" t="s">
+        <v>172</v>
+      </c>
+      <c r="H54" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
+        <v>54</v>
+      </c>
+      <c r="F56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="H57" s="21"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>46</v>
+      </c>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" t="s">
+        <v>94</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>96</v>
+      </c>
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>49</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F61" t="s">
         <v>97</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G61" t="s">
         <v>95</v>
       </c>
-      <c r="H53" s="22" t="s">
+      <c r="H61" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>68</v>
       </c>
-      <c r="H54" s="22"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" t="s">
+      <c r="H62" s="21"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+      <c r="B63" t="s">
         <v>69</v>
       </c>
-      <c r="H55" s="22"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" t="s">
+      <c r="H63" s="21"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" t="s">
         <v>46</v>
       </c>
-      <c r="H56" s="22"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="D57" t="s">
+      <c r="H64" s="21"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>140</v>
+      </c>
+      <c r="G65" t="s">
+        <v>172</v>
+      </c>
+      <c r="H65" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
         <v>49</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F66" t="s">
         <v>99</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G66" t="s">
         <v>98</v>
       </c>
-      <c r="H57" s="22" t="s">
+      <c r="H66" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="D58" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>22</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E67" t="s">
         <v>54</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F67" t="s">
         <v>101</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G67" t="s">
         <v>100</v>
       </c>
-      <c r="H58" s="22" t="s">
+      <c r="H67" s="21" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>140</v>
+      </c>
+      <c r="G70" t="s">
+        <v>172</v>
+      </c>
+      <c r="H70" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" t="s">
+        <v>166</v>
+      </c>
+      <c r="G71" t="s">
+        <v>164</v>
+      </c>
+      <c r="H71" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1837,6 +1986,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1B98F8-E09E-4DCF-A998-1D34528B2919}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -1940,7 +2129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E9C5AA-9540-45DB-BCC0-5EA98DDA6B0B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2004,7 +2193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2176,13 +2365,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,7 +2554,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
@@ -2376,10 +2565,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2387,32 +2576,32 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="C19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2420,57 +2609,90 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>135</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>136</v>
       </c>
-      <c r="C21" t="b">
+      <c r="C22" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
       </c>
+      <c r="D24" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
       <c r="C25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:C25">
-    <sortCondition ref="A23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A24:C28">
+    <sortCondition ref="A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to translations of warnings + vaccine names in CRIANCA
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F9CF5D-8052-4878-8F90-45A737EF2831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DFE38-F860-4658-9820-A279264326EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="175">
   <si>
     <t>setting_name</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>ACCIHOSP</t>
-  </si>
-  <si>
-    <t>Date of hospitalisation</t>
   </si>
   <si>
     <t>DATAINT</t>
@@ -480,9 +477,6 @@
     <t>display.constraint_message.text</t>
   </si>
   <si>
-    <t>Date of hospitalisation cannot be in the future</t>
-  </si>
-  <si>
     <t>Region: &lt;b&gt;{{data.reg}}&lt;b&gt;</t>
   </si>
   <si>
@@ -565,6 +559,15 @@
   </si>
   <si>
     <t>Comments to hospitalization</t>
+  </si>
+  <si>
+    <t>The date of hospitalization cannot be in the future</t>
+  </si>
+  <si>
+    <t>Date of hospitalization</t>
+  </si>
+  <si>
+    <t>A data da hospitalização não pode ser no futuro</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1169,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>23</v>
@@ -1174,10 +1177,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1193,9 +1196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,16 +1251,16 @@
         <v>30</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1268,13 +1271,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1283,16 +1286,16 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1301,7 +1304,7 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" s="21"/>
     </row>
@@ -1311,13 +1314,13 @@
         <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1333,7 +1336,7 @@
         <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8" s="21"/>
     </row>
@@ -1343,13 +1346,13 @@
         <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1375,13 +1378,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1389,22 +1392,22 @@
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>173</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M14" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="N14" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1423,76 +1426,76 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G18" t="s">
         <v>75</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="D21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" t="s">
         <v>132</v>
-      </c>
-      <c r="E21" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" t="s">
-        <v>133</v>
       </c>
       <c r="H21" s="21"/>
       <c r="K21" s="10"/>
@@ -1503,7 +1506,7 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H22" s="21"/>
       <c r="K22" s="10"/>
@@ -1511,14 +1514,14 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H23" s="21"/>
       <c r="I23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K23" s="10"/>
     </row>
@@ -1543,7 +1546,7 @@
         <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H26" s="21"/>
     </row>
@@ -1556,13 +1559,13 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1571,13 +1574,13 @@
         <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29" t="s">
         <v>75</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J29" s="10"/>
     </row>
@@ -1606,13 +1609,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1626,7 +1629,7 @@
         <v>64</v>
       </c>
       <c r="G34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H34" s="21" t="s">
         <v>62</v>
@@ -1649,7 +1652,7 @@
         <v>66</v>
       </c>
       <c r="G36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H36" s="21" t="s">
         <v>67</v>
@@ -1678,13 +1681,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1698,10 +1701,10 @@
         <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1721,10 +1724,10 @@
         <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1749,13 +1752,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1769,10 +1772,10 @@
         <v>77</v>
       </c>
       <c r="G48" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1820,13 +1823,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G54" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1840,10 +1843,10 @@
         <v>82</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1857,10 +1860,10 @@
         <v>83</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1877,13 +1880,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H59" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -1897,10 +1900,10 @@
         <v>84</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -1923,7 +1926,7 @@
         <v>85</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -1948,13 +1951,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H66" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -1968,7 +1971,7 @@
         <v>88</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -1985,7 +1988,7 @@
         <v>90</v>
       </c>
       <c r="H68" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2001,13 +2004,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H71" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2015,13 +2018,13 @@
         <v>49</v>
       </c>
       <c r="F72" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G72" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H72" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2096,10 +2099,10 @@
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2109,24 +2112,24 @@
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
         <v>121</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2282,82 +2285,82 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="str">
         <f>"8888"</f>
         <v>8888</v>
       </c>
       <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
         <v>138</v>
-      </c>
-      <c r="D9" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="str">
         <f>"9999"</f>
@@ -2444,7 +2447,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
@@ -2532,7 +2535,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2543,7 +2546,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
@@ -2554,7 +2557,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
@@ -2565,7 +2568,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
@@ -2576,7 +2579,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>49</v>
@@ -2587,10 +2590,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2598,10 +2601,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2631,10 +2634,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
         <v>124</v>
-      </c>
-      <c r="B22" t="s">
-        <v>125</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2642,7 +2645,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
         <v>60</v>
@@ -2651,12 +2654,12 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -2667,7 +2670,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
         <v>49</v>
@@ -2689,7 +2692,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Updates to a bit of everything
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E342FDB5-DCA3-4DA7-B9C3-34A41D231AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA581F-DF8E-4E6E-899F-20D2E5575EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="176">
   <si>
     <t>setting_name</t>
   </si>
@@ -334,9 +334,6 @@
     <t>informador</t>
   </si>
   <si>
-    <t>Special information - why was the interview not possible</t>
-  </si>
-  <si>
     <t>Inf</t>
   </si>
   <si>
@@ -350,12 +347,6 @@
   </si>
   <si>
     <t>Entrevista não possivel</t>
-  </si>
-  <si>
-    <t>data('informador') =='4'</t>
-  </si>
-  <si>
-    <t>data('informador') =='2'</t>
   </si>
   <si>
     <t>Who?</t>
@@ -568,6 +559,18 @@
   </si>
   <si>
     <t>adate.diffInDays(data('CONT'), data('DATAINT'))&lt;1 || adate.hasUncertainty(data('DATAINT'))</t>
+  </si>
+  <si>
+    <t>Why was the interview not possible</t>
+  </si>
+  <si>
+    <t>data('INFORMADOR') =='4'</t>
+  </si>
+  <si>
+    <t>data('INFORMADOR') =='2' || data('INFORMADOR') =='3'</t>
+  </si>
+  <si>
+    <t>data('INFORMADOR') !='4'</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1172,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>23</v>
@@ -1177,10 +1180,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,11 +1197,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,16 +1254,16 @@
         <v>30</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1271,13 +1274,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1286,10 +1289,10 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
         <v>99</v>
@@ -1304,7 +1307,7 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="H5" s="21"/>
     </row>
@@ -1314,13 +1317,13 @@
         <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1336,7 +1339,7 @@
         <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="H8" s="21"/>
     </row>
@@ -1346,13 +1349,13 @@
         <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1370,483 +1373,475 @@
       <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
       <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>128</v>
-      </c>
-      <c r="G13" t="s">
-        <v>156</v>
-      </c>
-      <c r="H13" t="s">
-        <v>157</v>
-      </c>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="G14" t="s">
-        <v>172</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="G15" t="s">
+        <v>169</v>
+      </c>
+      <c r="H15" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="L14" t="s">
-        <v>174</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="L15" t="s">
         <v>171</v>
       </c>
-      <c r="N14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" t="s">
+      <c r="M15" t="s">
+        <v>168</v>
+      </c>
+      <c r="N15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" t="s">
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G17" t="s">
-        <v>156</v>
-      </c>
-      <c r="H17" t="s">
-        <v>157</v>
-      </c>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>129</v>
+        <v>153</v>
+      </c>
+      <c r="H18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="D19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" t="s">
-        <v>148</v>
+        <v>75</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="G20" t="s">
-        <v>146</v>
-      </c>
-      <c r="H20" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="H20" t="s">
         <v>145</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H21" s="21"/>
-      <c r="K21" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="G21" t="s">
+        <v>143</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
         <v>133</v>
+      </c>
+      <c r="F22" t="s">
+        <v>129</v>
       </c>
       <c r="H22" s="21"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
-      <c r="D23" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23" t="s">
-        <v>93</v>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>130</v>
       </c>
       <c r="H23" s="21"/>
-      <c r="I23" t="s">
-        <v>139</v>
-      </c>
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" t="s">
+        <v>136</v>
+      </c>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" t="s">
+      <c r="H25" s="21"/>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" t="s">
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" t="s">
         <v>63</v>
       </c>
-      <c r="C26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" t="s">
-        <v>156</v>
-      </c>
-      <c r="H28" t="s">
-        <v>157</v>
-      </c>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
       <c r="D29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="G29" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="J29" s="10"/>
+        <v>153</v>
+      </c>
+      <c r="H29" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" t="s">
         <v>69</v>
-      </c>
-      <c r="H30" s="21"/>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" t="s">
-        <v>68</v>
       </c>
       <c r="H31" s="21"/>
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="21"/>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" t="s">
         <v>46</v>
       </c>
-      <c r="H32" s="21"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" t="s">
-        <v>156</v>
-      </c>
-      <c r="H33" t="s">
-        <v>157</v>
-      </c>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" t="s">
+        <v>153</v>
+      </c>
+      <c r="H34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>22</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>54</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>64</v>
       </c>
-      <c r="G34" t="s">
-        <v>159</v>
-      </c>
-      <c r="H34" s="21" t="s">
+      <c r="G35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H35" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>65</v>
       </c>
-      <c r="H35" s="21"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>49</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>66</v>
       </c>
-      <c r="G36" t="s">
-        <v>160</v>
-      </c>
-      <c r="H36" s="21" t="s">
+      <c r="G37" t="s">
+        <v>157</v>
+      </c>
+      <c r="H37" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="H37" s="21"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" t="s">
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" t="s">
         <v>69</v>
       </c>
-      <c r="H38" s="21"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" t="s">
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="H39" s="21"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>128</v>
-      </c>
-      <c r="G40" t="s">
-        <v>156</v>
-      </c>
-      <c r="H40" t="s">
-        <v>157</v>
-      </c>
+      <c r="E40" s="5"/>
+      <c r="H40" s="21"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>22</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>54</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>73</v>
       </c>
-      <c r="G41" t="s">
-        <v>161</v>
-      </c>
-      <c r="H41" s="21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="G42" t="s">
+        <v>158</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>63</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>74</v>
       </c>
-      <c r="H42" s="21"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+      <c r="H43" s="21"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
         <v>49</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>76</v>
       </c>
-      <c r="G43" t="s">
-        <v>162</v>
-      </c>
-      <c r="H43" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="G44" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>68</v>
       </c>
-      <c r="H44" s="21"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" t="s">
+      <c r="H45" s="21"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="21"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" t="s">
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="H46" s="21"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>128</v>
-      </c>
-      <c r="G47" t="s">
-        <v>156</v>
-      </c>
-      <c r="H47" t="s">
-        <v>157</v>
-      </c>
+      <c r="H47" s="21"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" t="s">
+        <v>153</v>
+      </c>
+      <c r="H48" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>22</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>54</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>77</v>
       </c>
-      <c r="G48" t="s">
-        <v>164</v>
-      </c>
-      <c r="H48" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="G49" t="s">
+        <v>161</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>63</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>78</v>
       </c>
-      <c r="H49" s="21"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+      <c r="H50" s="21"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>49</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>81</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" t="s">
         <v>80</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="H51" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>68</v>
       </c>
-      <c r="H51" s="21"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" t="s">
+      <c r="H52" s="21"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" t="s">
         <v>69</v>
       </c>
-      <c r="H52" s="21"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" t="s">
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="H53" s="21"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>128</v>
-      </c>
-      <c r="G54" t="s">
-        <v>156</v>
-      </c>
-      <c r="H54" t="s">
-        <v>157</v>
-      </c>
+      <c r="H54" s="21"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E55" t="s">
-        <v>54</v>
-      </c>
-      <c r="F55" t="s">
-        <v>82</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="H55" s="21" t="s">
-        <v>116</v>
+        <v>125</v>
+      </c>
+      <c r="G55" t="s">
+        <v>153</v>
+      </c>
+      <c r="H55" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1857,179 +1852,201 @@
         <v>54</v>
       </c>
       <c r="F56" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" t="s">
         <v>83</v>
       </c>
-      <c r="G56" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>69</v>
-      </c>
-      <c r="H57" s="21"/>
+      <c r="G57" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>46</v>
       </c>
-      <c r="H58" s="21"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G59" t="s">
-        <v>156</v>
-      </c>
-      <c r="H59" t="s">
-        <v>157</v>
-      </c>
+      <c r="H59" s="21"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
+        <v>125</v>
+      </c>
+      <c r="G60" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>22</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
         <v>54</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>84</v>
       </c>
-      <c r="G60" s="13" t="s">
+      <c r="G61" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>86</v>
+      </c>
+      <c r="H62" s="21"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" t="s">
+        <v>85</v>
+      </c>
+      <c r="H63" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="H60" s="21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" t="s">
-        <v>86</v>
-      </c>
-      <c r="H61" s="21"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>49</v>
-      </c>
-      <c r="F62" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62" t="s">
-        <v>85</v>
-      </c>
-      <c r="H62" s="21" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>68</v>
       </c>
-      <c r="H63" s="21"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" t="s">
+      <c r="H64" s="21"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+      <c r="B65" t="s">
         <v>69</v>
       </c>
-      <c r="H64" s="21"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" t="s">
+      <c r="H65" s="21"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" t="s">
         <v>46</v>
       </c>
-      <c r="H65" s="21"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>128</v>
-      </c>
-      <c r="G66" t="s">
-        <v>156</v>
-      </c>
-      <c r="H66" t="s">
-        <v>157</v>
-      </c>
+      <c r="H66" s="21"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>49</v>
-      </c>
-      <c r="F67" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="G67" t="s">
-        <v>88</v>
-      </c>
-      <c r="H67" s="21" t="s">
-        <v>97</v>
+        <v>153</v>
+      </c>
+      <c r="H67" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" t="s">
+        <v>89</v>
+      </c>
+      <c r="G68" t="s">
+        <v>88</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
         <v>22</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
         <v>54</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F69" t="s">
         <v>91</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G69" t="s">
         <v>90</v>
       </c>
-      <c r="H68" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" t="s">
+      <c r="H69" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>128</v>
-      </c>
-      <c r="G71" t="s">
-        <v>156</v>
-      </c>
-      <c r="H71" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
+        <v>125</v>
+      </c>
+      <c r="G72" t="s">
+        <v>153</v>
+      </c>
+      <c r="H72" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>49</v>
       </c>
-      <c r="F72" t="s">
-        <v>150</v>
-      </c>
-      <c r="G72" t="s">
-        <v>170</v>
-      </c>
-      <c r="H72" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="F73" t="s">
+        <v>147</v>
+      </c>
+      <c r="G73" t="s">
+        <v>167</v>
+      </c>
+      <c r="H73" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2099,10 +2116,10 @@
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2112,24 +2129,24 @@
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2213,7 +2230,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="A9:D10"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,82 +2302,82 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
+      <c r="C6" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>104</v>
+      <c r="C7" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C8" t="s">
-        <v>105</v>
+      <c r="C8" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B9" t="str">
         <f>"8888"</f>
         <v>8888</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B10" t="str">
         <f>"9999"</f>
@@ -2535,7 +2552,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2546,7 +2563,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
@@ -2557,7 +2574,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
@@ -2568,7 +2585,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
@@ -2593,7 +2610,7 @@
         <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2601,10 +2618,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2634,10 +2651,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2645,7 +2662,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
         <v>60</v>
@@ -2654,12 +2671,12 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -2670,7 +2687,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -2681,7 +2698,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
New qustions to hosp and campaign
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
+++ b/app/config/tables/CRIANCA_HOSP/forms/CRIANCA_HOSP/CRIANCA_HOSP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA581F-DF8E-4E6E-899F-20D2E5575EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE26F6-000C-4BFD-9FD6-0AE17CE19B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1201,7 +1201,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>